<commit_message>
feat: Add BOM diff tool
Add diff tool to identify added, removed, and quantity-changed items
Add ability to export to Excel or PDF
Refactor formatting with Prettier
</commit_message>
<xml_diff>
--- a/bom-samples/file_1.xlsx
+++ b/bom-samples/file_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Projects\BomItemConsolidater\bom-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD51DD2E-AEFD-43D5-A5BC-E32BB8D962B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5DA9B5-D444-425E-A7D7-749A3A75F090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="10515" windowWidth="29040" windowHeight="16440" tabRatio="483" xr2:uid="{C7D1D9F8-0418-4686-B826-B453F2DDAB5F}"/>
+    <workbookView xWindow="-18555" yWindow="6825" windowWidth="18660" windowHeight="13170" tabRatio="483" xr2:uid="{C7D1D9F8-0418-4686-B826-B453F2DDAB5F}"/>
   </bookViews>
   <sheets>
     <sheet name="file_1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="39">
   <si>
     <t>BILL OF MATERIAL</t>
   </si>
@@ -147,10 +147,13 @@
     <t>HD</t>
   </si>
   <si>
-    <t>A-D</t>
-  </si>
-  <si>
-    <t>A789783924507huktdfsuhksdfghjkhlsjkv89ypnf89p53fv79h979h3569q85eyops</t>
+    <t>lorem</t>
+  </si>
+  <si>
+    <t>eps</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -686,22 +689,22 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.69140625" style="1"/>
-    <col min="2" max="2" width="5.84375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.53515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="5.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="39" style="3" customWidth="1"/>
-    <col min="5" max="5" width="37.15234375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="100.53515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="20.3828125" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="100.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -711,7 +714,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -721,7 +724,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -741,15 +744,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="8">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
+      <c r="C4" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>37</v>
@@ -761,13 +764,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="8">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>17</v>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>12</v>
@@ -779,13 +782,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="70.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="8">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>13</v>
@@ -797,7 +800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -807,7 +810,7 @@
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
@@ -827,15 +830,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>17</v>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -847,13 +850,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="8">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>17</v>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>12</v>
@@ -865,13 +868,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="8">
         <v>2</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>17</v>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>13</v>
@@ -883,18 +886,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="8">
         <v>4</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>17</v>
+      <c r="C12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>26</v>
@@ -903,15 +906,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="8">
         <v>6</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>17</v>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>15</v>
@@ -923,15 +926,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="8">
         <v>2</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>17</v>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>16</v>
@@ -943,7 +946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
@@ -953,7 +956,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>1</v>
       </c>
@@ -973,15 +976,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="8">
         <v>6</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>17</v>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>11</v>
@@ -993,15 +996,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="8">
         <v>3</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>17</v>
+      <c r="C18" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>14</v>
@@ -1013,15 +1016,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="8">
         <v>6</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>17</v>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>15</v>
@@ -1033,15 +1036,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>17</v>
+      <c r="C20" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>16</v>
@@ -1053,15 +1056,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="8">
         <v>7</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>17</v>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -1073,15 +1076,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="8">
         <v>3</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>17</v>
+      <c r="C22" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>19</v>
@@ -1093,7 +1096,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1106,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
@@ -1123,15 +1126,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="8">
         <v>2</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>17</v>
+      <c r="C25" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>13</v>
@@ -1143,13 +1146,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="8">
         <v>3</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>17</v>
+      <c r="C26" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>16</v>
@@ -1161,15 +1164,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="8">
         <v>6</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>17</v>
+      <c r="C27" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>18</v>
@@ -1205,17 +1208,17 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.15234375" style="1"/>
-    <col min="2" max="2" width="5.84375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="5.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="39" style="3" customWidth="1"/>
-    <col min="4" max="4" width="37.15234375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="100.53515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="20.3828125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="100.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1227,7 @@
       <c r="D1" s="10"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1233,7 +1236,7 @@
       <c r="D2" s="10"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="8">
         <v>2</v>
@@ -1282,7 +1285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="8">
         <v>5</v>
@@ -1297,7 +1300,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1309,7 @@
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="8">
         <v>9</v>
@@ -1355,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="8">
         <v>2</v>
@@ -1370,7 +1373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
@@ -1430,7 +1433,7 @@
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1464,7 +1467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1515,7 +1518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>17</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
@@ -1558,7 +1561,7 @@
       <c r="D23" s="10"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>17</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="8">
         <v>3</v>
@@ -1607,7 +1610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>

</xml_diff>